<commit_message>
Push classify file scan updated fix bug
</commit_message>
<xml_diff>
--- a/all_pdf_keyword_counts.xlsx
+++ b/all_pdf_keyword_counts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -690,6 +690,126 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Công nghệ</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Đảm bảo</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Công việc</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Làm việc</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Chuyển đổi số</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Tra cứu</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PVP_Baocaothuongnien_2022.pdf</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Blockchain</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Push code json to excel
</commit_message>
<xml_diff>
--- a/all_pdf_keyword_counts.xlsx
+++ b/all_pdf_keyword_counts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,246 +570,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Công nghệ</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Đảm bảo</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Công việc</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Làm việc</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>AI</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Chuyển đổi số</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Tra cứu</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CMP_Baocaothuongnien_2021.pdf</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Blockchain</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Công nghệ</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Đảm bảo</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Công việc</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Làm việc</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>AI</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Chuyển đổi số</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Tra cứu</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>PVP_Baocaothuongnien_2022.pdf</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Blockchain</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>